<commit_message>
a little bit edit
</commit_message>
<xml_diff>
--- a/ggma_Business Reference Model.xlsx
+++ b/ggma_Business Reference Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="585" windowWidth="24015" windowHeight="10830"/>
+    <workbookView xWindow="630" yWindow="585" windowWidth="24015" windowHeight="10830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2017 1차" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="323">
   <si>
     <t>(정책목표)
 본부 단위 업무기능</t>
@@ -2353,10 +2353,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>대여</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>연구 및 자문</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -2386,6 +2382,23 @@
   </si>
   <si>
     <t>*경기기록아카이브2017로이동</t>
+  </si>
+  <si>
+    <t>답사단</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>워크숍</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>31개시군촬영</t>
+  </si>
+  <si>
+    <t>8개주제촬영</t>
+  </si>
+  <si>
+    <t>경기도주제작품</t>
   </si>
 </sst>
 </file>
@@ -2604,7 +2617,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2728,6 +2741,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3968,7 +3987,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="312">
+  <cellXfs count="313">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -4760,21 +4779,6 @@
     <xf numFmtId="0" fontId="28" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -4810,6 +4814,24 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -5127,17 +5149,17 @@
   </sheetPr>
   <dimension ref="A1:V1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="40.7109375" style="92" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" style="287" customWidth="1"/>
-    <col min="3" max="3" width="66.28515625" style="288" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="73.140625" style="289" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="66.28515625" style="288" customWidth="1"/>
+    <col min="4" max="4" width="73.140625" style="289" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="64.140625" style="290" customWidth="1"/>
     <col min="6" max="6" width="63.42578125" style="175" customWidth="1"/>
     <col min="7" max="7" width="61" style="291" customWidth="1"/>
@@ -5749,20 +5771,22 @@
       <c r="A20" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="300" t="s">
+      <c r="B20" s="295" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="301" t="s">
+      <c r="C20" s="296" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="302" t="s">
+      <c r="D20" s="297" t="s">
         <v>268</v>
       </c>
-      <c r="E20" s="303" t="s">
+      <c r="E20" s="298" t="s">
         <v>269</v>
       </c>
-      <c r="F20" s="304"/>
-      <c r="G20" s="305"/>
+      <c r="F20" s="299" t="s">
+        <v>318</v>
+      </c>
+      <c r="G20" s="300"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -5781,16 +5805,18 @@
     </row>
     <row r="21" spans="1:22" ht="41.25" thickBot="1">
       <c r="A21" s="100"/>
-      <c r="B21" s="306"/>
-      <c r="C21" s="307"/>
-      <c r="D21" s="308" t="s">
+      <c r="B21" s="301"/>
+      <c r="C21" s="302"/>
+      <c r="D21" s="303" t="s">
         <v>270</v>
       </c>
-      <c r="E21" s="309" t="s">
+      <c r="E21" s="304" t="s">
         <v>271</v>
       </c>
-      <c r="F21" s="310"/>
-      <c r="G21" s="311"/>
+      <c r="F21" s="305" t="s">
+        <v>319</v>
+      </c>
+      <c r="G21" s="306"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -6105,20 +6131,20 @@
       <c r="A31" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="295" t="s">
+      <c r="B31" s="307" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="296" t="s">
+      <c r="C31" s="308" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="297" t="s">
+      <c r="D31" s="309" t="s">
         <v>208</v>
       </c>
-      <c r="E31" s="298" t="s">
+      <c r="E31" s="310" t="s">
         <v>209</v>
       </c>
-      <c r="F31" s="299"/>
-      <c r="G31" s="123"/>
+      <c r="F31" s="311"/>
+      <c r="G31" s="312"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -6232,7 +6258,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="127" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C35" s="146" t="s">
         <v>131</v>
@@ -6804,7 +6830,7 @@
         <v>205</v>
       </c>
       <c r="F53" s="258" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G53" s="126"/>
       <c r="H53" s="1"/>
@@ -6834,7 +6860,7 @@
         <v>172</v>
       </c>
       <c r="F54" s="258" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G54" s="126"/>
       <c r="H54" s="1"/>
@@ -6864,7 +6890,7 @@
         <v>173</v>
       </c>
       <c r="F55" s="258" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G55" s="126"/>
       <c r="H55" s="1"/>
@@ -6894,7 +6920,7 @@
         <v>174</v>
       </c>
       <c r="F56" s="274" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G56" s="141"/>
       <c r="H56" s="1"/>
@@ -6926,8 +6952,8 @@
       <c r="D57" s="234" t="s">
         <v>195</v>
       </c>
-      <c r="E57" s="283">
-        <v>31</v>
+      <c r="E57" s="283" t="s">
+        <v>320</v>
       </c>
       <c r="F57" s="258"/>
       <c r="G57" s="126"/>
@@ -6950,14 +6976,14 @@
     <row r="58" spans="1:22">
       <c r="A58" s="102"/>
       <c r="B58" s="121" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C58" s="161"/>
       <c r="D58" s="234" t="s">
         <v>196</v>
       </c>
-      <c r="E58" s="284">
-        <v>8</v>
+      <c r="E58" s="284" t="s">
+        <v>321</v>
       </c>
       <c r="F58" s="258"/>
       <c r="G58" s="126"/>
@@ -6973,20 +6999,20 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="1:22">
-      <c r="A59" s="102"/>
-      <c r="B59" s="121" t="s">
-        <v>315</v>
-      </c>
-      <c r="C59" s="161"/>
-      <c r="D59" s="234" t="s">
+    <row r="59" spans="1:22" ht="21" thickBot="1">
+      <c r="A59" s="110"/>
+      <c r="B59" s="150" t="s">
+        <v>314</v>
+      </c>
+      <c r="C59" s="162"/>
+      <c r="D59" s="285" t="s">
         <v>197</v>
       </c>
-      <c r="E59" s="284" t="s">
-        <v>310</v>
-      </c>
-      <c r="F59" s="258"/>
-      <c r="G59" s="126"/>
+      <c r="E59" s="286" t="s">
+        <v>322</v>
+      </c>
+      <c r="F59" s="274"/>
+      <c r="G59" s="141"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -7020,7 +7046,7 @@
     </row>
     <row r="61" spans="1:22">
       <c r="A61" s="294" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B61" s="174"/>
       <c r="C61" s="177"/>
@@ -29700,11 +29726,11 @@
   </sheetPr>
   <dimension ref="A1:AB97"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C58" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -32552,7 +32578,7 @@
     </row>
     <row r="88" spans="1:28" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A88" s="293" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="1:28" s="6" customFormat="1" ht="15.75" customHeight="1"/>

</xml_diff>